<commit_message>
feature: add objective, precondition
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\PycharmProjects\teko-import-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABC\PycharmProjects\teko-import-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,36 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>Test case name</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>d</t>
+    <t>OBJECTIVE</t>
+  </si>
+  <si>
+    <t>PRECONDITION</t>
+  </si>
+  <si>
+    <t>Return HTTP 400 when input is invalid</t>
+  </si>
+  <si>
+    <t>Test validate input</t>
+  </si>
+  <si>
+    <t>No precondition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,52 +359,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: handle \n in file excel
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -41,7 +41,8 @@
     <t>Test validate input</t>
   </si>
   <si>
-    <t>No precondition</t>
+    <t>Condition 1
+Condition 2</t>
   </si>
 </sst>
 </file>
@@ -77,8 +78,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,14 +366,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -383,14 +387,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>